<commit_message>
adjust the module for model diagnostic, change the visuals to plotlies, add lines where appropriate, and att limits to facilitate better interpretation of the plots.
</commit_message>
<xml_diff>
--- a/Dependencies/templates.xlsx
+++ b/Dependencies/templates.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QuantyFeyApplication for Publication\QuantyFey\Dependencies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08F25C4-25E2-4A64-AA5F-03D4F7111C16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B30D498-A05F-4ECC-8BA0-A6B8EF7603EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{C0122184-1F29-479A-8613-AD1D5913AF83}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="2" xr2:uid="{C0122184-1F29-479A-8613-AD1D5913AF83}"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
     <sheet name="ExampleAllCompounds" sheetId="2" r:id="rId2"/>
+    <sheet name="Alexandra" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Concentration</t>
   </si>
@@ -128,6 +129,21 @@
   </si>
   <si>
     <t>Cadaverin_2xderiv_373.1_280.01_quant</t>
+  </si>
+  <si>
+    <t>stnd300</t>
+  </si>
+  <si>
+    <t>stnd100</t>
+  </si>
+  <si>
+    <t>stnd30</t>
+  </si>
+  <si>
+    <t>stnd10</t>
+  </si>
+  <si>
+    <t>stnd3</t>
   </si>
 </sst>
 </file>
@@ -571,7 +587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAF7D3D-C491-4764-BB66-AE2B39F8CCBE}">
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -1225,4 +1241,67 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECA82E5-AA2E-4331-9361-163C1C808343}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>3.3333333333333335E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed names of transitions in Example 2 dataset cahnged respective names in tempalte.xlsx added an additional pane for upload of different tempalte.xlsx file
</commit_message>
<xml_diff>
--- a/Dependencies/templates.xlsx
+++ b/Dependencies/templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QuantyFeyApplication for Publication\QuantyFey\Dependencies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338737F0-6DBA-46A1-9B80-2E879D3C52D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE022C4A-9543-4FAB-915A-AA9974700059}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{C0122184-1F29-479A-8613-AD1D5913AF83}"/>
   </bookViews>
@@ -55,51 +55,6 @@
     <t>Cal.Name</t>
   </si>
   <si>
-    <t>Lysine_147_84_DP_50_CE_30_quan</t>
-  </si>
-  <si>
-    <t>Proline_116.1_70_DP_50_CE_25_quan</t>
-  </si>
-  <si>
-    <t>Ornitine_133.1_70_DP_40_CE_30_quan</t>
-  </si>
-  <si>
-    <t>Trigonelline_138_92_DP_60_CE_30_quan</t>
-  </si>
-  <si>
-    <t>Methionine_150_104.1_DP_60_CE_15_quan</t>
-  </si>
-  <si>
-    <t>Guanine_152_135_DP_60_CE_30_quan</t>
-  </si>
-  <si>
-    <t>Xanthine_153_110_DP_60_CE_30_quan</t>
-  </si>
-  <si>
-    <t>Histidine_156.1_110_DP_60_CE_20_quan</t>
-  </si>
-  <si>
-    <t>Carnitine_162.1_103_DP_60_CE_25_quan</t>
-  </si>
-  <si>
-    <t>Phenylalanine_166.1_120_DP_50_CE_22_quan</t>
-  </si>
-  <si>
-    <t>MethionineSulfoxide_166.1_74_DP_50_CE_20_quan</t>
-  </si>
-  <si>
-    <t>Spermidine_203.2_98_DP_60_CE_35_quan</t>
-  </si>
-  <si>
-    <t>Tryptophan_205.1_188.1_DP_50_CE_15_quan</t>
-  </si>
-  <si>
-    <t>Kynurenine_209.1_192_DP_60_CE_15_quan</t>
-  </si>
-  <si>
-    <t>Thyroxine_777.7_731.7_DP_100_CE_35_quan</t>
-  </si>
-  <si>
     <t>HILIC Cal 8</t>
   </si>
   <si>
@@ -124,55 +79,100 @@
     <t>HILIC Cal 1</t>
   </si>
   <si>
-    <t>Serine_104_74.1_DP_.50_CE_.15_quan</t>
-  </si>
-  <si>
-    <t>Inol_225.1_44.9_DP_.30_CE_.45_quan</t>
-  </si>
-  <si>
-    <t>Acetyl.Ornitine_175.1_115_DP_50_CE_20_quan</t>
-  </si>
-  <si>
-    <t>Homo.Arginine_189.1_144_DP_60_CE_23_quan</t>
-  </si>
-  <si>
-    <t>Isoleucine.Leucine_132.1_69_DP_50_CE_25_quan</t>
-  </si>
-  <si>
-    <t>AC.C2_204.1_85.1_DP_50_CE_27_quan</t>
-  </si>
-  <si>
-    <t>AC.C3_218.1_85.1_DP_50_CE_29_quan</t>
-  </si>
-  <si>
-    <t>AC.C4_232.2_85.1_DP_50_CE_29_quan</t>
-  </si>
-  <si>
-    <t>AC.C5.1_244.2_85.1_DP_50_CE_31_quan</t>
-  </si>
-  <si>
-    <t>AC.C5_246.2_85.1_DP_50_CE_29_quan</t>
-  </si>
-  <si>
-    <t>AC.C6_260.2_85.1_DP_50_CE_33_quan</t>
-  </si>
-  <si>
-    <t>Asparagine_131_114_DP_.50_CE_.15_quan</t>
-  </si>
-  <si>
-    <t>AR.PyroGlu_130_84_DP_60_CE_20_quan</t>
-  </si>
-  <si>
-    <t>X1.Methyl.Histidine_170.1_124_DP_55_CE_20_quan</t>
-  </si>
-  <si>
-    <t>X3.Methyl.Histidine_170.1_96_DP_60_CE_28_quan</t>
-  </si>
-  <si>
-    <t>AR.ADMA_203.2_70_DP_60_CE_40_quan</t>
-  </si>
-  <si>
-    <t>AC.C5.DC._276.2_85.1_DP_61_CE_35_quan</t>
+    <t>Serine_104_74.1_DP_.50_CE_.15_quant</t>
+  </si>
+  <si>
+    <t>Asparagine_131_114_DP_.50_CE_.15_quant</t>
+  </si>
+  <si>
+    <t>Inol_225.1_44.9_DP_.30_CE_.45_quant</t>
+  </si>
+  <si>
+    <t>Lysine_147_84_DP_50_CE_30_quant</t>
+  </si>
+  <si>
+    <t>Proline_116.1_70_DP_50_CE_25_quant</t>
+  </si>
+  <si>
+    <t>AR.PyroGlu_130_84_DP_60_CE_20_quant</t>
+  </si>
+  <si>
+    <t>Ornitine_133.1_70_DP_40_CE_30_quant</t>
+  </si>
+  <si>
+    <t>Trigonelline_138_92_DP_60_CE_30_quant</t>
+  </si>
+  <si>
+    <t>Methionine_150_104.1_DP_60_CE_15_quant</t>
+  </si>
+  <si>
+    <t>Guanine_152_135_DP_60_CE_30_quant</t>
+  </si>
+  <si>
+    <t>Xanthine_153_110_DP_60_CE_30_quant</t>
+  </si>
+  <si>
+    <t>Histidine_156.1_110_DP_60_CE_20_quant</t>
+  </si>
+  <si>
+    <t>Carnitine_162.1_103_DP_60_CE_25_quant</t>
+  </si>
+  <si>
+    <t>Phenylalanine_166.1_120_DP_50_CE_22_quant</t>
+  </si>
+  <si>
+    <t>MethionineSulfoxide_166.1_74_DP_50_CE_20_quant</t>
+  </si>
+  <si>
+    <t>X1.Methyl.Histidine_170.1_124_DP_55_CE_20_quant</t>
+  </si>
+  <si>
+    <t>X3.Methyl.Histidine_170.1_96_DP_60_CE_28_quant</t>
+  </si>
+  <si>
+    <t>Acetyl.Ornitine_175.1_115_DP_50_CE_20_quant</t>
+  </si>
+  <si>
+    <t>Homo.Arginine_189.1_144_DP_60_CE_23_quant</t>
+  </si>
+  <si>
+    <t>AR.ADMA_203.2_70_DP_60_CE_40_quant</t>
+  </si>
+  <si>
+    <t>Spermidine_203.2_98_DP_60_CE_35_quant</t>
+  </si>
+  <si>
+    <t>AC.C2_204.1_85.1_DP_50_CE_27_quant</t>
+  </si>
+  <si>
+    <t>Tryptophan_205.1_188.1_DP_50_CE_15_quant</t>
+  </si>
+  <si>
+    <t>Kynurenine_209.1_192_DP_60_CE_15_quant</t>
+  </si>
+  <si>
+    <t>AC.C3_218.1_85.1_DP_50_CE_29_quant</t>
+  </si>
+  <si>
+    <t>AC.C4_232.2_85.1_DP_50_CE_29_quant</t>
+  </si>
+  <si>
+    <t>AC.C5.1_244.2_85.1_DP_50_CE_31_quant</t>
+  </si>
+  <si>
+    <t>AC.C5_246.2_85.1_DP_50_CE_29_quant</t>
+  </si>
+  <si>
+    <t>AC.C6_260.2_85.1_DP_50_CE_33_quant</t>
+  </si>
+  <si>
+    <t>AC.C5.DC._276.2_85.1_DP_61_CE_35_quant</t>
+  </si>
+  <si>
+    <t>Thyroxine_777.7_731.7_DP_100_CE_35_quant</t>
+  </si>
+  <si>
+    <t>Isoleucine.Leucine_132.1_69_DP_50_CE_25_quant</t>
   </si>
 </sst>
 </file>
@@ -628,7 +628,7 @@
   <dimension ref="A1:AH9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,55 +638,55 @@
         <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>34</v>
@@ -695,49 +695,49 @@
         <v>35</v>
       </c>
       <c r="U1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="AH1" s="1"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3">
         <v>3</v>
@@ -839,7 +839,7 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3">
         <v>10</v>
@@ -941,7 +941,7 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3">
         <v>30</v>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3">
         <v>100</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3">
         <v>300</v>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3">
         <v>1000</v>
@@ -1349,7 +1349,7 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3">
         <v>3000</v>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3">
         <v>10000</v>

</xml_diff>